<commit_message>
december data generated, swtiched to gmaps, visualised with folio
</commit_message>
<xml_diff>
--- a/raw data/flats_available.xlsx
+++ b/raw data/flats_available.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yeelongsiah/Desktop/Personal/PythonLearning/PPHS/raw data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4652AA7E-EFA7-E54F-8459-8A180DAD9F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3F9262-BBCA-B14E-8B74-4FFC6155CFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{F1963D34-0239-8748-ADC1-ECD068EEB2BC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{F1963D34-0239-8748-ADC1-ECD068EEB2BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="77">
   <si>
     <t>-</t>
   </si>
@@ -47,9 +47,6 @@
     <t> Bedok</t>
   </si>
   <si>
-    <t> Blk 13 Bedok South Road</t>
-  </si>
-  <si>
     <t> -</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t> Blk 3 Tiong Bahru Road</t>
   </si>
   <si>
-    <t>4Q2027</t>
-  </si>
-  <si>
     <t> Blk 5 Tiong Bahru Road</t>
   </si>
   <si>
@@ -80,15 +74,9 @@
     <t> Blk 55 Lengkok Bahru</t>
   </si>
   <si>
-    <t> Blk 115 Jalan Bukit Merah</t>
-  </si>
-  <si>
     <t> Choa Chu Kang</t>
   </si>
   <si>
-    <t> Blk 9 Teck Whye Lane</t>
-  </si>
-  <si>
     <t>- </t>
   </si>
   <si>
@@ -107,12 +95,6 @@
     <t> Blk 967B Jurong West Street 93</t>
   </si>
   <si>
-    <t>Kallang/ Whampoa </t>
-  </si>
-  <si>
-    <t> Queenstown</t>
-  </si>
-  <si>
     <t> Sembawang</t>
   </si>
   <si>
@@ -134,27 +116,9 @@
     <t> Blk 63 Lorong 5 Toa Payoh</t>
   </si>
   <si>
-    <t>Woodlands</t>
-  </si>
-  <si>
     <t> Blk 147 Woodlands Street 13</t>
   </si>
   <si>
-    <t> Blk 153 Woodlands Street 13</t>
-  </si>
-  <si>
-    <t> Yishun</t>
-  </si>
-  <si>
-    <t> Blk 510A Yishun Street 51</t>
-  </si>
-  <si>
-    <t> Blk 510B Yishun Street 51</t>
-  </si>
-  <si>
-    <t> Blk 70 Commonwealth Drive</t>
-  </si>
-  <si>
     <t> Blk 462 Sembawang Drive</t>
   </si>
   <si>
@@ -185,21 +149,9 @@
     <t>months_to_expiry</t>
   </si>
   <si>
-    <t> Ang Mo Kio</t>
-  </si>
-  <si>
-    <t> Blk 629 Ang Mo Kio Avenue 4</t>
-  </si>
-  <si>
     <t> Blk 113 Bedok North Street 2</t>
   </si>
   <si>
-    <t> Bishan</t>
-  </si>
-  <si>
-    <t> Blk 410 Sin Ming Avenue</t>
-  </si>
-  <si>
     <t> Blk 435A Bukit Batok West Avenue 5</t>
   </si>
   <si>
@@ -212,46 +164,109 @@
     <t> Blk 31 Telok Blangah Rise</t>
   </si>
   <si>
-    <t> Blk 110 Jalan Bukit Merah</t>
-  </si>
-  <si>
-    <t> Blk 116 Jalan Bukit Merah</t>
-  </si>
-  <si>
-    <t> Blk 121 Bukit Merah Lane 1</t>
-  </si>
-  <si>
     <t> Blk 813A Choa Chu Kang Avenue 7</t>
   </si>
   <si>
-    <t> Marine Parade</t>
-  </si>
-  <si>
-    <t> Blk 52 Marine Terrace</t>
-  </si>
-  <si>
     <t> Blk 4 Dover Road</t>
   </si>
   <si>
-    <t> Blk 83 Commonwealth Close</t>
-  </si>
-  <si>
     <t> Blk 693D Woodlands Avenue 6</t>
   </si>
   <si>
     <t> Blk 785A Woodlands Rise</t>
   </si>
   <si>
-    <t> Blk 108 Yishun Ring Road</t>
-  </si>
-  <si>
     <t> Blk 313 Hougang Avenue 5</t>
   </si>
   <si>
-    <t> Blk 1 Thomson Road</t>
-  </si>
-  <si>
     <t> Blk 144 Woodlands Street 13</t>
+  </si>
+  <si>
+    <t>4Q 2028</t>
+  </si>
+  <si>
+    <t> Blk 556 Bedok North Street 3</t>
+  </si>
+  <si>
+    <t> Blk 119 Bukit Merah Lane 1</t>
+  </si>
+  <si>
+    <t> Clementi</t>
+  </si>
+  <si>
+    <t> Blk 501 West Coast Drive</t>
+  </si>
+  <si>
+    <t> Geylang</t>
+  </si>
+  <si>
+    <t> Blk 1 Haig Road</t>
+  </si>
+  <si>
+    <t> Blk 3 Haig Road</t>
+  </si>
+  <si>
+    <t> Blk 13 Old Airport Road</t>
+  </si>
+  <si>
+    <t> Blk 52 Cassia Crescent</t>
+  </si>
+  <si>
+    <t> Blk 25 Hougang Avenue 3</t>
+  </si>
+  <si>
+    <t> Blk 191 Boon Lay Drive</t>
+  </si>
+  <si>
+    <t>Kallang/Whampoa </t>
+  </si>
+  <si>
+    <t> Blk 7 St. George's Lane</t>
+  </si>
+  <si>
+    <t> Blk 45 Bendemeer Road</t>
+  </si>
+  <si>
+    <t>Queenstown</t>
+  </si>
+  <si>
+    <t> Blk 350 Anchorvale Road</t>
+  </si>
+  <si>
+    <t> Blk 463A Sengkang West Way</t>
+  </si>
+  <si>
+    <t> Blk 463B Sengkang West Way</t>
+  </si>
+  <si>
+    <t> Blk 3 Upper Aljunied Lane</t>
+  </si>
+  <si>
+    <t> Blk 68 Lorong 5 Toa Payoh</t>
+  </si>
+  <si>
+    <t> Blk 110 Lorong 1 Toa Payoh</t>
+  </si>
+  <si>
+    <t> Blk 116 Lorong 2 Toa Payoh</t>
+  </si>
+  <si>
+    <t> Blk 146 Potong Pasir Avenue 1</t>
+  </si>
+  <si>
+    <t> Woodlands</t>
+  </si>
+  <si>
+    <t> Blk 180C Marsiling Road</t>
+  </si>
+  <si>
+    <t> Blk 316 Hougang Avenue 5</t>
+  </si>
+  <si>
+    <t> Blk 188 Boon Lay Drive</t>
+  </si>
+  <si>
+    <t> Blk 967A Jurong West Street 93</t>
   </si>
 </sst>
 </file>
@@ -287,9 +302,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,74 +640,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{810E8CB9-AD67-394A-9E44-CC6CFF6E9EA2}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="192" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="136" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>45</v>
+        <v>30</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="H1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="G2" s="1">
         <f>DATE(RIGHT(F2,4),LEFT(F2,1)*3,1)</f>
-        <v>47543</v>
+        <v>47088</v>
       </c>
       <c r="H2">
         <f ca="1">DATEDIF(TODAY(),G2,"m")</f>
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -699,83 +713,83 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G42" si="0">DATE(RIGHT(F3,4),LEFT(F3,1)*3,1)</f>
-        <v>46722</v>
+        <f t="shared" ref="G3:G49" si="0">DATE(RIGHT(F3,4),LEFT(F3,1)*3,1)</f>
+        <v>47543</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H42" ca="1" si="1">DATEDIF(TODAY(),G3,"m")</f>
-        <v>37</v>
+        <f t="shared" ref="H3:H49" ca="1" si="1">DATEDIF(TODAY(),G3,"m")</f>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>46722</v>
+        <v>47543</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>46722</v>
+        <v>47088</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -783,27 +797,27 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>0</v>
+      <c r="E6" s="2">
+        <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>47543</v>
+        <v>46357</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -811,19 +825,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
@@ -831,55 +845,55 @@
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
         <v>2</v>
       </c>
-      <c r="E8">
-        <v>7</v>
+      <c r="E8" s="2">
+        <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>46357</v>
+        <v>46722</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9">
+        <v>40</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
         <v>4</v>
       </c>
-      <c r="E9">
-        <v>5</v>
+      <c r="E9" s="2">
+        <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
@@ -887,27 +901,27 @@
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
@@ -915,80 +929,80 @@
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>46722</v>
+        <v>47543</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="0"/>
-        <v>46722</v>
+        <v>47543</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>17</v>
+        <v>50</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="F13" t="s">
         <v>1</v>
@@ -999,23 +1013,23 @@
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="s">
@@ -1027,23 +1041,23 @@
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="s">
@@ -1055,23 +1069,23 @@
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="s">
@@ -1083,23 +1097,23 @@
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="s">
@@ -1111,23 +1125,23 @@
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="s">
@@ -1139,79 +1153,76 @@
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19">
-        <v>9</v>
-      </c>
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="2">
+        <v>2</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="0"/>
-        <v>46722</v>
+        <v>47543</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s">
-        <v>0</v>
-      </c>
-      <c r="E20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="0"/>
-        <v>47543</v>
+        <v>47088</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>6</v>
-      </c>
-      <c r="E21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="s">
@@ -1223,24 +1234,24 @@
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>13</v>
-      </c>
-      <c r="E22" t="s">
-        <v>0</v>
+        <v>74</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
+        <v>4</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="F22" t="s">
         <v>1</v>
@@ -1251,23 +1262,23 @@
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23">
-        <v>11</v>
-      </c>
-      <c r="E23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="2">
+        <v>10</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="s">
@@ -1279,51 +1290,51 @@
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>0</v>
-      </c>
-      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
+        <v>24</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" si="0"/>
-        <v>46722</v>
+        <v>47543</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="2">
+        <v>9</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="s">
@@ -1335,79 +1346,79 @@
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="2">
+        <v>41</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G26" s="1">
         <f t="shared" si="0"/>
-        <v>46722</v>
+        <v>47543</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27" t="s">
-        <v>0</v>
-      </c>
-      <c r="E27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="2">
+        <v>3</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G27" s="1">
         <f t="shared" si="0"/>
-        <v>46722</v>
+        <v>47543</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F28" t="s">
@@ -1419,51 +1430,51 @@
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
-        <v>0</v>
-      </c>
-      <c r="E29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="G29" s="1">
         <f t="shared" si="0"/>
-        <v>46722</v>
+        <v>47088</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>0</v>
-      </c>
-      <c r="E30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F30" t="s">
@@ -1475,164 +1486,164 @@
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31" t="s">
-        <v>0</v>
-      </c>
-      <c r="E31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="G31" s="1">
         <f t="shared" si="0"/>
-        <v>47543</v>
+        <v>47088</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32">
-        <v>2</v>
-      </c>
-      <c r="D32" t="s">
-        <v>0</v>
-      </c>
-      <c r="E32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G32" s="1">
         <f t="shared" si="0"/>
-        <v>46722</v>
+        <v>47543</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33">
-        <v>4</v>
-      </c>
-      <c r="D33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="2">
+        <v>3</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G33" s="1">
         <f t="shared" si="0"/>
-        <v>46722</v>
+        <v>47543</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34">
-        <v>15</v>
-      </c>
-      <c r="D34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="2">
+        <v>3</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="G34" s="1">
         <f t="shared" si="0"/>
-        <v>46722</v>
+        <v>47088</v>
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
-      </c>
-      <c r="C35" t="s">
-        <v>0</v>
-      </c>
-      <c r="D35" t="s">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>32</v>
+        <v>64</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="G35" s="1">
         <f t="shared" si="0"/>
-        <v>47543</v>
+        <v>47088</v>
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" t="s">
-        <v>0</v>
-      </c>
-      <c r="D36" t="s">
-        <v>0</v>
-      </c>
-      <c r="E36">
-        <v>21</v>
+        <v>65</v>
+      </c>
+      <c r="C36" s="2">
+        <v>6</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F36" t="s">
         <v>1</v>
@@ -1643,24 +1654,24 @@
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37" t="s">
-        <v>0</v>
-      </c>
-      <c r="D37" t="s">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>4</v>
+        <v>66</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F37" t="s">
         <v>1</v>
@@ -1671,23 +1682,23 @@
       </c>
       <c r="H37">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38">
-        <v>2</v>
-      </c>
-      <c r="D38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F38" t="s">
@@ -1699,80 +1710,80 @@
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>67</v>
-      </c>
-      <c r="C39">
-        <v>7</v>
-      </c>
-      <c r="D39" t="s">
-        <v>0</v>
-      </c>
-      <c r="E39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="G39" s="1">
         <f t="shared" si="0"/>
-        <v>47543</v>
+        <v>47088</v>
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B40" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40" t="s">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="2">
+        <v>5</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="G40" s="1">
         <f t="shared" si="0"/>
-        <v>47543</v>
+        <v>47088</v>
       </c>
       <c r="H40">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41" t="s">
-        <v>0</v>
-      </c>
-      <c r="E41" t="s">
-        <v>0</v>
+        <v>68</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2">
+        <v>1</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F41" t="s">
         <v>1</v>
@@ -1783,35 +1794,231 @@
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B42" t="s">
-        <v>37</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E42" t="s">
-        <v>0</v>
+        <v>69</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2">
+        <v>1</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="F42" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G42" s="1">
         <f t="shared" si="0"/>
-        <v>46722</v>
+        <v>47543</v>
       </c>
       <c r="H42">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="2">
+        <v>1</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" si="0"/>
+        <v>47543</v>
+      </c>
+      <c r="H43">
+        <f t="shared" ca="1" si="1"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2">
+        <v>1</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>1</v>
+      </c>
+      <c r="G44" s="1">
+        <f t="shared" si="0"/>
+        <v>47543</v>
+      </c>
+      <c r="H44">
+        <f t="shared" ca="1" si="1"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2">
+        <v>11</v>
+      </c>
+      <c r="F45" t="s">
+        <v>1</v>
+      </c>
+      <c r="G45" s="1">
+        <f t="shared" si="0"/>
+        <v>47543</v>
+      </c>
+      <c r="H45">
+        <f t="shared" ca="1" si="1"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" s="2">
+        <v>2</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1</v>
+      </c>
+      <c r="G46" s="1">
+        <f t="shared" si="0"/>
+        <v>47543</v>
+      </c>
+      <c r="H46">
+        <f t="shared" ca="1" si="1"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" s="2">
+        <v>1</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1</v>
+      </c>
+      <c r="G47" s="1">
+        <f t="shared" si="0"/>
+        <v>47543</v>
+      </c>
+      <c r="H47">
+        <f t="shared" ca="1" si="1"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48" s="2">
+        <v>1</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>1</v>
+      </c>
+      <c r="G48" s="1">
+        <f t="shared" si="0"/>
+        <v>47543</v>
+      </c>
+      <c r="H48">
+        <f t="shared" ca="1" si="1"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" s="2">
+        <v>1</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>1</v>
+      </c>
+      <c r="G49" s="1">
+        <f t="shared" si="0"/>
+        <v>47543</v>
+      </c>
+      <c r="H49">
+        <f t="shared" ca="1" si="1"/>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>